<commit_message>
New Updates for the user and User Service Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/displayName.xlsx
+++ b/src/test/resources/displayName.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="100">
   <si>
     <t>Long-Term Issuer Default Rating Action</t>
   </si>
@@ -187,6 +187,135 @@
   </si>
   <si>
     <t>Support Rating Floor Watch/Outlook</t>
+  </si>
+  <si>
+    <t>Fund Quality Rating Action</t>
+  </si>
+  <si>
+    <t>Fund Quality Effective Date</t>
+  </si>
+  <si>
+    <t>Fund Quality Rating Watch/Outlook</t>
+  </si>
+  <si>
+    <t>Fund Quality Rating Solicitation Status</t>
+  </si>
+  <si>
+    <t>Investment Management Quality Rating</t>
+  </si>
+  <si>
+    <t>Investment Management Quality Rating Action</t>
+  </si>
+  <si>
+    <t>Investment Management Quality Rating Effective Date</t>
+  </si>
+  <si>
+    <t>Investment Management Quality Rating Watch/Outlook</t>
+  </si>
+  <si>
+    <t>Investment Management Quality Rating Solicitation Status</t>
+  </si>
+  <si>
+    <t>National Investment Management Quality Rating</t>
+  </si>
+  <si>
+    <t>National Investment Management Quality Rating Action</t>
+  </si>
+  <si>
+    <t>National Investment Management Quality Rating Effective Date</t>
+  </si>
+  <si>
+    <t>National Investment Management Quality Rating Watch/Outlook</t>
+  </si>
+  <si>
+    <t>National Investment Management Quality Rating Solicitation Status</t>
+  </si>
+  <si>
+    <t>Most recent CMBS Special Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Last relevant activity of the associated rating</t>
+  </si>
+  <si>
+    <t>Calendar date and 24-hour time from when the associated rating took effect</t>
+  </si>
+  <si>
+    <t>Indicates the assoaciated rating’s status on Rating Watch or Rating Outlook</t>
+  </si>
+  <si>
+    <t>Associated rating solicited by buy-side, sell-side, or unsolicited</t>
+  </si>
+  <si>
+    <t>Most recent CMBS Primary Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent CMBS Master Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Special Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - Home Equity Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - High LTV Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - Sub Prime Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - Alt A Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - Prime Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Master Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent ABS Special Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent ABS Master Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent ABS Primary Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent ABS Seller/Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent Servicer Rating (Primary) for non-conforming RMBS [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent Servicer Rating (Special) for non-conforming RMBS [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - Specialty (reverse mortgage) [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent CMBS Construction Loan Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer - Subservicer [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Specialty Servicer - Option ARMS [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Specialty Servicer - Second Liens [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent Small Balance Commercial Primary Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent Small Balance Commercial Special Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent RMBS Primary Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
+  </si>
+  <si>
+    <t>Most recent CMBS Large Loan Special Servicer Rating [+ rating suffix (parenthesised) where applicable]</t>
   </si>
 </sst>
 </file>
@@ -249,13 +378,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:A196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,6 +982,701 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>